<commit_message>
C - Updated current workflow ---- A- new test files
</commit_message>
<xml_diff>
--- a/MerchantNew/ExcelReader/MerchantApp.xlsx
+++ b/MerchantNew/ExcelReader/MerchantApp.xlsx
@@ -2,28 +2,28 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="702" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="702" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCase" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="PrepaidRecharge" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="RetailerLogin" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="PostpaidRecharge" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="DthRecharge" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="MahanagarGasRecharge" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="RelianceElectricity" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="DelhiJalBoardRecharge" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="BsnlRecharge" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="TestCase" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="PrepaidRecharge" r:id="rId3" sheetId="2" state="visible"/>
+    <sheet name="RetailerLogin" r:id="rId4" sheetId="3" state="visible"/>
+    <sheet name="PostpaidRecharge" r:id="rId5" sheetId="4" state="visible"/>
+    <sheet name="DthRecharge" r:id="rId6" sheetId="5" state="visible"/>
+    <sheet name="MahanagarGasRecharge" r:id="rId7" sheetId="6" state="visible"/>
+    <sheet name="RelianceElectricity" r:id="rId8" sheetId="7" state="visible"/>
+    <sheet name="DelhiJalBoardRecharge" r:id="rId9" sheetId="8" state="visible"/>
+    <sheet name="BsnlRecharge" r:id="rId10" sheetId="9" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="35">
   <si>
     <t>TCID</t>
   </si>
@@ -46,18 +46,21 @@
     <t>N</t>
   </si>
   <si>
+    <t>Skip</t>
+  </si>
+  <si>
     <t>PrepaidRecharge</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>PostpaidRecharge</t>
   </si>
   <si>
     <t>DthRecharge</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>MahanagarGasRecharge</t>
   </si>
   <si>
@@ -119,6 +122,12 @@
   </si>
   <si>
     <t>02</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Error while doing DTH Recharge</t>
   </si>
 </sst>
 </file>
@@ -180,14 +189,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="hair"/>
       <right style="hair"/>
       <top style="hair"/>
@@ -196,71 +205,93 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="15">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -270,21 +301,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="C16" activeCellId="0" pane="topLeft" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.1734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="23.6122448979592" collapsed="true"/>
+    <col min="2" max="3" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
+    <col min="5" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -301,7 +332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -309,90 +340,94 @@
         <v>6</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="14" t="s">
+        <v>33</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -405,26 +440,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="27.72265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
+    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -433,42 +468,46 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -481,23 +520,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -506,19 +545,19 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -526,22 +565,22 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -554,26 +593,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.1275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.1734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="9.58673469387755" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="39.1275510204082" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
+    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -582,42 +621,42 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -630,23 +669,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -655,48 +694,48 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -709,28 +748,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.1734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="11.9489795918367" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
+    <col min="4" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="17.1071428571429" collapsed="true"/>
+    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -739,48 +778,48 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>21</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -793,25 +832,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="F17" activeCellId="0" pane="topLeft" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col min="1" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="17.1071428571429" collapsed="true"/>
+    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -820,48 +859,48 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -874,23 +913,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -899,42 +938,42 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -947,23 +986,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -972,42 +1011,42 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
U- updated the code
</commit_message>
<xml_diff>
--- a/MerchantNew/ExcelReader/MerchantApp.xlsx
+++ b/MerchantNew/ExcelReader/MerchantApp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="702" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="5" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="702" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" r:id="rId2" sheetId="1" state="visible"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="36">
   <si>
     <t>TCID</t>
   </si>
@@ -46,88 +46,91 @@
     <t>N</t>
   </si>
   <si>
+    <t>PrepaidRecharge</t>
+  </si>
+  <si>
+    <t>PostpaidRecharge</t>
+  </si>
+  <si>
+    <t>DthRecharge</t>
+  </si>
+  <si>
+    <t>MahanagarGasRecharge</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>RelianceElectricity</t>
+  </si>
+  <si>
+    <t>DelhiJalBoardRecharge</t>
+  </si>
+  <si>
+    <t>BsnlRecharge</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Error while doing DTH Recharge</t>
+  </si>
+  <si>
+    <t>9819042543</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>9967903705</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>3000000000</t>
+  </si>
+  <si>
+    <t>CA Number</t>
+  </si>
+  <si>
+    <t>Bill No</t>
+  </si>
+  <si>
+    <t>210000651086</t>
+  </si>
+  <si>
+    <t>Cycle No</t>
+  </si>
+  <si>
     <t>Skip</t>
   </si>
   <si>
-    <t>PrepaidRecharge</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>PostpaidRecharge</t>
-  </si>
-  <si>
-    <t>DthRecharge</t>
-  </si>
-  <si>
-    <t>MahanagarGasRecharge</t>
-  </si>
-  <si>
-    <t>RelianceElectricity</t>
-  </si>
-  <si>
-    <t>DelhiJalBoardRecharge</t>
-  </si>
-  <si>
-    <t>BsnlRecharge</t>
-  </si>
-  <si>
-    <t>Actual Result</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>9819042543</t>
-  </si>
-  <si>
-    <t>12345</t>
-  </si>
-  <si>
-    <t>9967903705</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Customer ID</t>
-  </si>
-  <si>
-    <t>3000000000</t>
-  </si>
-  <si>
-    <t>CA Number</t>
-  </si>
-  <si>
-    <t>Bill No</t>
-  </si>
-  <si>
-    <t>210000651086</t>
-  </si>
-  <si>
-    <t>Cycle No</t>
-  </si>
-  <si>
     <t>152285924</t>
   </si>
   <si>
     <t>02</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Error while doing DTH Recharge</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -229,7 +232,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -250,21 +253,35 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="true"/>
@@ -304,7 +321,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="C16" activeCellId="0" pane="topLeft" sqref="C16"/>
+      <selection activeCell="B6" activeCellId="0" pane="topLeft" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -340,41 +357,37 @@
         <v>6</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D2" s="4"/>
       <c r="E2" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+      <c r="A4" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
-      <c r="A4" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="6"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
-      <c r="A5" s="5" t="s">
-        <v>11</v>
+      <c r="A5" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -382,13 +395,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="7"/>
       <c r="E6" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
@@ -396,10 +411,12 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
@@ -407,10 +424,12 @@
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
@@ -418,10 +437,12 @@
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="3"/>
     </row>
   </sheetData>
@@ -442,15 +463,15 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="27.72265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="27.7295918367347" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
     <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
@@ -482,26 +503,26 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -565,16 +586,16 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -637,20 +658,20 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -706,30 +727,30 @@
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -750,15 +771,15 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="11.9489795918367" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="11.953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
     <col min="4" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
     <col min="8" max="8" hidden="false" style="0" width="17.1071428571429" collapsed="true"/>
     <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
@@ -787,33 +808,37 @@
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -835,12 +860,15 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="F17" activeCellId="0" pane="topLeft" sqref="F17"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="11.953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
+    <col min="4" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
     <col min="8" max="8" hidden="false" style="0" width="17.1071428571429" collapsed="true"/>
     <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
@@ -868,33 +896,37 @@
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -916,12 +948,15 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="11.953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
+    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -952,22 +987,26 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -989,12 +1028,15 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="11.953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
+    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -1025,22 +1067,26 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Code Based on New Flow
</commit_message>
<xml_diff>
--- a/MerchantNew/ExcelReader/MerchantApp.xlsx
+++ b/MerchantNew/ExcelReader/MerchantApp.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="758" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" tabRatio="758" windowHeight="8190" windowWidth="16380" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCase" r:id="rId2" sheetId="1" state="visible"/>
-    <sheet name="PrepaidRecharge" r:id="rId3" sheetId="2" state="visible"/>
-    <sheet name="RetailerLogin" r:id="rId4" sheetId="3" state="visible"/>
-    <sheet name="PostpaidRecharge" r:id="rId5" sheetId="4" state="visible"/>
-    <sheet name="DthRecharge" r:id="rId6" sheetId="5" state="visible"/>
-    <sheet name="MahanagarGasRecharge" r:id="rId7" sheetId="6" state="visible"/>
-    <sheet name="BsnlRecharge" r:id="rId8" sheetId="7" state="visible"/>
-    <sheet name="RelianceElectricity" r:id="rId9" sheetId="8" state="visible"/>
-    <sheet name="DelhiJalBoardRecharge" r:id="rId10" sheetId="9" state="visible"/>
-    <sheet name="AddRetailer" r:id="rId11" sheetId="10" state="visible"/>
-    <sheet name="AddDistributor" r:id="rId12" sheetId="11" state="visible"/>
+    <sheet name="TestCase" r:id="rId1" sheetId="1"/>
+    <sheet name="PrepaidRecharge" r:id="rId2" sheetId="2"/>
+    <sheet name="RetailerLogin" r:id="rId3" sheetId="3"/>
+    <sheet name="PostpaidRecharge" r:id="rId4" sheetId="4"/>
+    <sheet name="DthRecharge" r:id="rId5" sheetId="5"/>
+    <sheet name="MahanagarGasRecharge" r:id="rId6" sheetId="6"/>
+    <sheet name="BsnlRecharge" r:id="rId7" sheetId="7"/>
+    <sheet name="RelianceElectricity" r:id="rId8" sheetId="8"/>
+    <sheet name="DelhiJalBoardRecharge" r:id="rId9" sheetId="9"/>
+    <sheet name="AddRetailer" r:id="rId10" sheetId="10"/>
+    <sheet name="AddDistributor" r:id="rId11" sheetId="11"/>
   </sheets>
-  <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="58">
   <si>
     <t>TCID</t>
   </si>
@@ -108,9 +107,6 @@
     <t>10</t>
   </si>
   <si>
-    <t>Sucessfully Logged into Application</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -196,16 +192,20 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Unable to Access Login Page and Get Login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -214,24 +214,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Monospace"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -264,87 +248,94 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -378,86 +369,325 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr lastClr="000000" val="windowText"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT h="25400" w="63500"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="D2" activeCellId="0" pane="topLeft" sqref="D2:D5"/>
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="D10" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="23.6122448979592" collapsed="true"/>
-    <col min="2" max="3" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
-    <col min="5" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" width="23.5703125" collapsed="true"/>
+    <col min="2" max="3" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.68359375" collapsed="true"/>
+    <col min="5" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -482,10 +712,12 @@
         <v>6</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
+      <c r="D2" s="36" t="s">
+        <v>22</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -496,7 +728,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -507,7 +739,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -518,7 +750,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -526,12 +758,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="33" t="s">
-        <v>28</v>
-      </c>
+      <c r="D6" s="17"/>
       <c r="E6" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -539,12 +769,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="D7" s="11"/>
       <c r="E7" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -552,12 +780,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="30" t="s">
-        <v>22</v>
-      </c>
+      <c r="D8" s="14"/>
       <c r="E8" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
+    <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -565,12 +791,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="36" t="s">
-        <v>22</v>
-      </c>
+      <c r="D9" s="20"/>
       <c r="E9" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
+    <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -578,10 +802,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="7"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -593,10 +817,9 @@
       <c r="E11" s="3"/>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" useFirstPageNumber="1" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -604,27 +827,24 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="J3" activeCellId="1" pane="topLeft" sqref="D2:D5 J3"/>
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="J3" activeCellId="1" sqref="D2:D5 J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="11.9489795918367" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
-    <col min="4" max="6" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="15.9744897959184" collapsed="true"/>
-    <col min="8" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="12.0" collapsed="true"/>
+    <col min="3" max="3" width="6.140625" collapsed="true"/>
+    <col min="4" max="6" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" width="16.0" collapsed="true"/>
+    <col min="8" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -638,68 +858,67 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row ht="51" r="2" spans="1:11">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="2">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="ajinka@ajinkya" r:id="rId1" ref="G2"/>
+    <hyperlink r:id="rId1" ref="G2"/>
   </hyperlinks>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -707,22 +926,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="J2" activeCellId="1" pane="topLeft" sqref="D2:D5 J2"/>
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="J2" activeCellId="1" sqref="D2:D5 J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,60 +952,59 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="2">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="ajinka@ajinkya" r:id="rId1" ref="G2"/>
+    <hyperlink r:id="rId1" ref="G2"/>
   </hyperlinks>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -797,25 +1012,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="1" pane="topLeft" sqref="D2:D5 B2"/>
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="B2" activeCellId="1" sqref="D2:D5 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="27.7295918367347" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="27.7109375" collapsed="true"/>
+    <col min="3" max="3" width="6.140625" collapsed="true"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -841,7 +1053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row ht="25.5" r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -866,10 +1078,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -877,25 +1088,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="1" pane="topLeft" sqref="D2:D5 B2"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="30.5459183673469" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="40.375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.68359375" collapsed="true"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -921,22 +1129,22 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>28</v>
+      <c r="B2" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
+      <c r="F2" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
@@ -946,10 +1154,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -957,25 +1164,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="1" pane="topLeft" sqref="D2:D5 B2"/>
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="B2" activeCellId="1" sqref="D2:D5 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="9.58673469387755" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="37.2602040816326" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" width="9.5703125" collapsed="true"/>
+    <col min="2" max="2" width="37.28515625" collapsed="true"/>
+    <col min="3" max="3" width="6.140625" collapsed="true"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1001,15 +1205,15 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row ht="25.5" r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
@@ -1026,10 +1230,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1037,25 +1240,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="F2" activeCellId="1" pane="topLeft" sqref="D2:D5 F2"/>
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="F2" activeCellId="1" sqref="D2:D5 F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="27.7295918367347" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="27.7109375" collapsed="true"/>
+    <col min="3" max="3" width="6.140625" collapsed="true"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1081,10 +1281,10 @@
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row ht="25.5" r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1108,14 +1308,13 @@
         <v>26</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1123,27 +1322,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="F29" activeCellId="1" pane="topLeft" sqref="D2:D5 F29"/>
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="F29" activeCellId="1" sqref="D2:D5 F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="24.3046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
-    <col min="4" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="17.1071428571429" collapsed="true"/>
-    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
+    <col min="4" max="7" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" width="17.140625" collapsed="true"/>
+    <col min="9" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1166,21 +1362,21 @@
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="2">
+    </row>
+    <row ht="25.5" r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>28</v>
+      <c r="B2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
@@ -1193,17 +1389,16 @@
         <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>35</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1211,25 +1406,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="F2" activeCellId="1" pane="topLeft" sqref="D2:D5 F2"/>
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="F2" activeCellId="1" sqref="D2:D5 F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="11.953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1255,14 +1447,14 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="2">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="34" t="s">
+      <c r="B2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="3"/>
@@ -1280,10 +1472,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1291,27 +1482,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="F2" activeCellId="1" pane="topLeft" sqref="D2:D5 F2"/>
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="F2" activeCellId="1" sqref="D2:D5 F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="24.3046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
-    <col min="4" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="17.1071428571429" collapsed="true"/>
-    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
+    <col min="4" max="7" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" width="17.140625" collapsed="true"/>
+    <col min="9" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1334,21 +1522,21 @@
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row ht="25.5" r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>28</v>
+      <c r="B2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
@@ -1361,17 +1549,16 @@
         <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>38</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1379,25 +1566,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="F2" activeCellId="1" pane="topLeft" sqref="D2:D5 F2"/>
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+      <selection activeCell="F2" activeCellId="1" sqref="D2:D5 F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="11.953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1422,18 +1606,18 @@
       <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="2">
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="3"/>
@@ -1449,15 +1633,14 @@
       <c r="H2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>40</v>
+      <c r="I2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Changed the folder and added the path variable
</commit_message>
<xml_diff>
--- a/MerchantNew/ExcelReader/MerchantApp.xlsx
+++ b/MerchantNew/ExcelReader/MerchantApp.xlsx
@@ -4,27 +4,27 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="2" tabRatio="758" windowHeight="8190" windowWidth="16380" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="758"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCase" r:id="rId1" sheetId="1"/>
-    <sheet name="PrepaidRecharge" r:id="rId2" sheetId="2"/>
-    <sheet name="RetailerLogin" r:id="rId3" sheetId="3"/>
-    <sheet name="PostpaidRecharge" r:id="rId4" sheetId="4"/>
-    <sheet name="DthRecharge" r:id="rId5" sheetId="5"/>
-    <sheet name="MahanagarGasRecharge" r:id="rId6" sheetId="6"/>
-    <sheet name="BsnlRecharge" r:id="rId7" sheetId="7"/>
-    <sheet name="RelianceElectricity" r:id="rId8" sheetId="8"/>
-    <sheet name="DelhiJalBoardRecharge" r:id="rId9" sheetId="9"/>
-    <sheet name="AddRetailer" r:id="rId10" sheetId="10"/>
-    <sheet name="AddDistributor" r:id="rId11" sheetId="11"/>
+    <sheet name="TestCase" sheetId="1" r:id="rId1"/>
+    <sheet name="PrepaidRecharge" sheetId="2" r:id="rId2"/>
+    <sheet name="RetailerLogin" sheetId="3" r:id="rId3"/>
+    <sheet name="PostpaidRecharge" sheetId="4" r:id="rId4"/>
+    <sheet name="DthRecharge" sheetId="5" r:id="rId5"/>
+    <sheet name="MahanagarGasRecharge" sheetId="6" r:id="rId6"/>
+    <sheet name="BsnlRecharge" sheetId="7" r:id="rId7"/>
+    <sheet name="RelianceElectricity" sheetId="8" r:id="rId8"/>
+    <sheet name="DelhiJalBoardRecharge" sheetId="9" r:id="rId9"/>
+    <sheet name="AddRetailer" sheetId="10" r:id="rId10"/>
+    <sheet name="AddDistributor" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="55">
   <si>
     <t>TCID</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Successfully Done PostPaidMobile Recharge</t>
-  </si>
-  <si>
     <t>Customer ID</t>
   </si>
   <si>
@@ -192,19 +189,12 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>Unable to Access Login Page and Get Login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -272,112 +262,85 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
+  <cellXfs count="28">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -391,10 +354,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -552,7 +515,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -561,13 +524,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -577,7 +540,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -586,7 +549,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -595,7 +558,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -605,12 +568,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -641,7 +604,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -660,7 +623,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -672,19 +635,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
-      <selection activeCell="D10" sqref="D2:D10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" collapsed="true"/>
-    <col min="2" max="3" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.68359375" collapsed="true"/>
-    <col min="5" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23.5703125" collapsed="1"/>
+    <col min="2" max="3" width="11.5703125" collapsed="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -712,9 +675,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="36" t="s">
-        <v>22</v>
-      </c>
+      <c r="D2" s="24"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5">
@@ -725,7 +686,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5">
@@ -817,8 +778,8 @@
       <c r="E11" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" useFirstPageNumber="1" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -827,21 +788,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="J3" activeCellId="1" sqref="D2:D5 J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" width="12.0" collapsed="true"/>
-    <col min="3" max="3" width="6.140625" collapsed="true"/>
-    <col min="4" max="6" width="11.5703125" collapsed="true"/>
-    <col min="7" max="7" width="16.0" collapsed="true"/>
-    <col min="8" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="1"/>
+    <col min="2" max="2" width="12" collapsed="1"/>
+    <col min="3" max="3" width="6.140625" collapsed="1"/>
+    <col min="4" max="6" width="11.5703125" collapsed="1"/>
+    <col min="7" max="7" width="16" collapsed="1"/>
+    <col min="8" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -858,66 +819,66 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="51">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row ht="51" r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -926,16 +887,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="J2" activeCellId="1" sqref="D2:D5 J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -952,22 +913,22 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -980,30 +941,30 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1012,19 +973,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
-      <selection activeCell="B2" activeCellId="1" sqref="D2:D5 B2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" width="27.7109375" collapsed="true"/>
-    <col min="3" max="3" width="6.140625" collapsed="true"/>
-    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1053,22 +1014,22 @@
         <v>20</v>
       </c>
     </row>
-    <row ht="25.5" r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="38.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="25" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
+      <c r="F2" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
@@ -1078,8 +1039,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1088,19 +1049,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="40.375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.68359375" collapsed="true"/>
-    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1133,18 +1094,14 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>22</v>
-      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>34</v>
+      <c r="F2" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
@@ -1154,8 +1111,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1164,19 +1121,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
-      <selection activeCell="B2" activeCellId="1" sqref="D2:D5 B2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" collapsed="true"/>
-    <col min="2" max="2" width="37.28515625" collapsed="true"/>
-    <col min="3" max="3" width="6.140625" collapsed="true"/>
-    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="9.5703125" collapsed="1"/>
+    <col min="2" max="2" width="37.28515625" collapsed="1"/>
+    <col min="3" max="3" width="6.140625" collapsed="1"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1205,16 +1162,12 @@
         <v>20</v>
       </c>
     </row>
-    <row ht="25.5" r="2" spans="1:8">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
         <v>23</v>
@@ -1230,8 +1183,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1240,19 +1193,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
-      <selection activeCell="F2" activeCellId="1" sqref="D2:D5 F2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" width="27.7109375" collapsed="true"/>
-    <col min="3" max="3" width="6.140625" collapsed="true"/>
-    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="1"/>
+    <col min="2" max="2" width="27.7109375" collapsed="1"/>
+    <col min="3" max="3" width="6.140625" collapsed="1"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1281,19 +1234,15 @@
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row ht="25.5" r="2" spans="1:9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
         <v>23</v>
@@ -1308,12 +1257,12 @@
         <v>26</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1322,21 +1271,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
-      <selection activeCell="F29" activeCellId="1" sqref="D2:D5 F29"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
-    <col min="4" max="7" width="11.5703125" collapsed="true"/>
-    <col min="8" max="8" width="17.140625" collapsed="true"/>
-    <col min="9" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="7" width="11.5703125" collapsed="1"/>
+    <col min="8" max="8" width="17.140625" collapsed="1"/>
+    <col min="9" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1362,22 +1311,18 @@
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row ht="25.5" r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>27</v>
-      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
         <v>23</v>
@@ -1389,15 +1334,15 @@
         <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>34</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1406,19 +1351,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F2" activeCellId="1" sqref="D2:D5 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
-    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1452,7 +1397,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>22</v>
@@ -1472,8 +1417,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1482,21 +1427,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F2" activeCellId="1" sqref="D2:D5 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
-    <col min="4" max="7" width="11.5703125" collapsed="true"/>
-    <col min="8" max="8" width="17.140625" collapsed="true"/>
-    <col min="9" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="7" width="11.5703125" collapsed="1"/>
+    <col min="8" max="8" width="17.140625" collapsed="1"/>
+    <col min="9" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1522,18 +1467,18 @@
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row ht="25.5" r="2" spans="1:9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="25.5">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>27</v>
@@ -1549,15 +1494,15 @@
         <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>37</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1566,19 +1511,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F2" activeCellId="1" sqref="D2:D5 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
-    <col min="4" max="1025" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="1025" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1607,7 +1552,7 @@
         <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1615,7 +1560,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>22</v>
@@ -1634,12 +1579,12 @@
         <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
-  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>